<commit_message>
Included SAGA C++ MR results..
git-svn-id: file://localhost/tmp/svn2git/svn@4054 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/applications/MapReduce/branches/MapReduce_Python/results/Python_Local_MR_results.xlsx
+++ b/applications/MapReduce/branches/MapReduce_Python/results/Python_Local_MR_results.xlsx
@@ -22,7 +22,275 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
+  <si>
+    <t>sierra</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>No of node assigned for map subjob</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>No of node assigned for reduce subjob</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sierra</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>The execution time increased linearly along with the input size. The Reduce Phase took maximum time as the number of subjobs used for reduce phase is 1.  The word count application requries the reduce  to be 1.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>As the number of workers vary for the same input file the execution time decreased. But the decrease is not substantial as the reduce phase is a bottle neck for word count</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>As the chunk size vary the execution time increased.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>For 64 MB the number of chunks for 1GB input file is 16 and the available workers are 8. So there is a queue waiting time involved</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>in processing 16 map chunks.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sierra</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying input Datasize</t>
+  </si>
+  <si>
+    <t>OLD-MR</t>
+  </si>
+  <si>
+    <t>INDIA</t>
+  </si>
+  <si>
+    <t>Wordcount</t>
+  </si>
+  <si>
+    <t>8 workers, 64 mb chunk</t>
+  </si>
+  <si>
+    <t>8 reduces</t>
+  </si>
+  <si>
+    <t>Input Data size(MB)</t>
+  </si>
+  <si>
+    <t>Master  Time to create sesion in advert</t>
+  </si>
+  <si>
+    <t>Chunk phase</t>
+  </si>
+  <si>
+    <t>SAGA C++ Mapreduce time to solution</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>it was changed to move and both time &amp; space are saved….</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1st run with single file</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analysis:</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>What more can be done?</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Workers</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-&gt;8</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>word count application counts the number of occurences of a word in the given input data.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input FileSize</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time to Start workers)</t>
+  </si>
+  <si>
+    <t>Prepare input files for reducer</t>
+  </si>
+  <si>
+    <t>Time to shutdown workers(sec)</t>
+  </si>
+  <si>
+    <t>New MR</t>
+  </si>
+  <si>
+    <t>Python MR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sierra </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sierra</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time sec</t>
+  </si>
+  <si>
+    <t>Reduce Phase Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map phase Time </t>
+  </si>
+  <si>
+    <t>Time taken to chunk files</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Map subjobs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of reduce jobs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>data which is taken but not used for representation as these tests are not valid..</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description:</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">As there 11 files and each file( size ~393MB ) generates 2 chunks. So totally they generated 23 chunk files.  </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>At a time only 8 files can be processed as there are only 8 subjobs for each phase.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Transfer</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sierra</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of total nodes requested for map / partition</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>No of node assigned for map</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>No of node assigned for reduce</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of total node requested for reduced</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time</t>
+  </si>
+  <si>
+    <t>Chunk size</t>
+  </si>
+  <si>
+    <t>64 MB</t>
+  </si>
+  <si>
+    <t>Infrastructure used</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sierra grid</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Application used</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>wordcount</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machines Used for Input,map,reduce,output</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sierra</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size of files transferred</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Map subjobs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of reduce jobs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machines Used for Input,map,reduce,output</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of total nodes requested for map / partition</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Infrastructure used</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sierra grid</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Application used</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>wordcount</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data obtained from www.freebase.com</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of input files</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
   <si>
     <t xml:space="preserve">For 128 &amp; 256  the performance is better and almost same. </t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -90,270 +358,6 @@
   <si>
     <t xml:space="preserve">The File Transfer from temp directory to output directory is local and the time is reduced drastically if files are moved instead of copy… The file transfer column contains time taken to copy… but later </t>
     <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>it was changed to move and both time &amp; space are saved….</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1st run with single file</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Analysis:</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>What more can be done?</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Workers</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-&gt;8</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>word count application counts the number of occurences of a word in the given input data.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input FileSize</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time to Start workers)</t>
-  </si>
-  <si>
-    <t>Prepare input files for reducer</t>
-  </si>
-  <si>
-    <t>Time to shutdown workers(sec)</t>
-  </si>
-  <si>
-    <t>New MR</t>
-  </si>
-  <si>
-    <t>Python MR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sierra </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time sec</t>
-  </si>
-  <si>
-    <t>Reduce Phase Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Map phase Time </t>
-  </si>
-  <si>
-    <t>Time taken to chunk files</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of Map subjobs</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of reduce jobs</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>data which is taken but not used for representation as these tests are not valid..</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description:</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">As there 11 files and each file( size ~393MB ) generates 2 chunks. So totally they generated 23 chunk files.  </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>At a time only 8 files can be processed as there are only 8 subjobs for each phase.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Transfer</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of total nodes requested for map / partition</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>No of node assigned for map</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>No of node assigned for reduce</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of total node requested for reduced</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time</t>
-  </si>
-  <si>
-    <t>Chunk size</t>
-  </si>
-  <si>
-    <t>64 MB</t>
-  </si>
-  <si>
-    <t>Infrastructure used</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra grid</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Application used</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>wordcount</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machines Used for Input,map,reduce,output</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Size of files transferred</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of Map subjobs</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of reduce jobs</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machines Used for Input,map,reduce,output</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of total nodes requested for map / partition</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Infrastructure used</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra grid</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Application used</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>wordcount</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data obtained from www.freebase.com</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of input files</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>No of node assigned for map subjob</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>No of node assigned for reduce subjob</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>The execution time increased linearly along with the input size. The Reduce Phase took maximum time as the number of subjobs used for reduce phase is 1.  The word count application requries the reduce  to be 1.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>As the number of workers vary for the same input file the execution time decreased. But the decrease is not substantial as the reduce phase is a bottle neck for word count</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>As the chunk size vary the execution time increased.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>For 64 MB the number of chunks for 1GB input file is 16 and the available workers are 8. So there is a queue waiting time involved</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>in processing 16 map chunks.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sierra</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying input Datasize</t>
-  </si>
-  <si>
-    <t>OLD-MR</t>
-  </si>
-  <si>
-    <t>INDIA</t>
-  </si>
-  <si>
-    <t>Wordcount</t>
-  </si>
-  <si>
-    <t>8 workers, 64 mb chunk</t>
-  </si>
-  <si>
-    <t>8 reduces</t>
-  </si>
-  <si>
-    <t>Input Data size(MB)</t>
-  </si>
-  <si>
-    <t>Master  Time to create sesion in advert</t>
-  </si>
-  <si>
-    <t>Chunk phase</t>
   </si>
 </sst>
 </file>
@@ -637,7 +641,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -918,11 +921,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="465946056"/>
-        <c:axId val="465944328"/>
+        <c:axId val="558904984"/>
+        <c:axId val="537559784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="465946056"/>
+        <c:axId val="558904984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,18 +946,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="465944328"/>
+        <c:crossAx val="537559784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="465944328"/>
+        <c:axId val="537559784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -976,11 +978,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="465946056"/>
+        <c:crossAx val="558904984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -991,6 +992,170 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>C++ MR, 8 workers, 256 Chunk Size, 8 reduces, 1 single input file</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>"C++ MR Exec time "</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$49:$B$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$Q$49:$Q$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>619.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>656.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>974.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1210.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="473222216"/>
+        <c:axId val="473225384"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="473222216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Input file size in MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="473225384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="473225384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time taken for execution in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="473222216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1024,7 +1189,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -1202,11 +1366,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="466004552"/>
-        <c:axId val="466016312"/>
+        <c:axId val="538825688"/>
+        <c:axId val="537125400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="466004552"/>
+        <c:axId val="538825688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,17 +1391,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466016312"/>
+        <c:crossAx val="537125400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="466016312"/>
+        <c:axId val="537125400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,18 +1422,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466004552"/>
+        <c:crossAx val="538825688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1303,7 +1464,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -1547,11 +1707,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="466061384"/>
-        <c:axId val="466068776"/>
+        <c:axId val="538277864"/>
+        <c:axId val="540202024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="466061384"/>
+        <c:axId val="538277864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,18 +1732,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466068776"/>
+        <c:crossAx val="540202024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="466068776"/>
+        <c:axId val="540202024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1605,18 +1764,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466061384"/>
+        <c:crossAx val="538277864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1779,11 +1936,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="502503912"/>
-        <c:axId val="502583928"/>
+        <c:axId val="537754248"/>
+        <c:axId val="536995896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="502503912"/>
+        <c:axId val="537754248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,14 +1965,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="502583928"/>
+        <c:crossAx val="536995896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="502583928"/>
+        <c:axId val="536995896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,7 +1998,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="502503912"/>
+        <c:crossAx val="537754248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2011,11 +2168,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="512560408"/>
-        <c:axId val="512532472"/>
+        <c:axId val="537020712"/>
+        <c:axId val="537282232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="512560408"/>
+        <c:axId val="537020712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,14 +2197,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512532472"/>
+        <c:crossAx val="537282232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="512532472"/>
+        <c:axId val="537282232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2073,7 +2230,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512560408"/>
+        <c:crossAx val="537020712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2231,11 +2388,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="503292872"/>
-        <c:axId val="513040312"/>
+        <c:axId val="538089464"/>
+        <c:axId val="538087512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="503292872"/>
+        <c:axId val="538089464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,14 +2417,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="513040312"/>
+        <c:crossAx val="538087512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="513040312"/>
+        <c:axId val="538087512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2293,7 +2450,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="503292872"/>
+        <c:crossAx val="538089464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2451,11 +2608,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="512946872"/>
-        <c:axId val="513114680"/>
+        <c:axId val="536581976"/>
+        <c:axId val="537758200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="512946872"/>
+        <c:axId val="536581976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,14 +2637,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="513114680"/>
+        <c:crossAx val="537758200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="513114680"/>
+        <c:axId val="537758200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2513,7 +2670,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512946872"/>
+        <c:crossAx val="536581976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2641,11 +2798,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="513521608"/>
-        <c:axId val="513218232"/>
+        <c:axId val="537092472"/>
+        <c:axId val="537101048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="513521608"/>
+        <c:axId val="537092472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2669,14 +2826,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="513218232"/>
+        <c:crossAx val="537101048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="513218232"/>
+        <c:axId val="537101048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2702,7 +2859,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="513521608"/>
+        <c:crossAx val="537092472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2884,11 +3041,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="497564696"/>
-        <c:axId val="497567864"/>
+        <c:axId val="536505112"/>
+        <c:axId val="537702616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497564696"/>
+        <c:axId val="536505112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2913,14 +3070,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497567864"/>
+        <c:crossAx val="537702616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497567864"/>
+        <c:axId val="537702616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2946,7 +3103,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497564696"/>
+        <c:crossAx val="536505112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3237,6 +3394,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3577,62 +3764,62 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="71" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3661,7 +3848,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J6">
         <v>8</v>
@@ -3705,7 +3892,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J7">
         <v>8</v>
@@ -3749,7 +3936,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J8">
         <v>8</v>
@@ -3793,7 +3980,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J9">
         <v>8</v>
@@ -3837,7 +4024,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J10">
         <v>8</v>
@@ -3857,7 +4044,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="D35" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -3886,7 +4073,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -3930,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J41">
         <v>2</v>
@@ -3974,7 +4161,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J42">
         <v>3</v>
@@ -4018,7 +4205,7 @@
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J43">
         <v>4</v>
@@ -4062,7 +4249,7 @@
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J44">
         <v>5</v>
@@ -4106,7 +4293,7 @@
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J45">
         <v>6</v>
@@ -4150,7 +4337,7 @@
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J46">
         <v>7</v>
@@ -4194,7 +4381,7 @@
         <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J47">
         <v>8</v>
@@ -4214,7 +4401,7 @@
     </row>
     <row r="71" spans="1:14">
       <c r="C71" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -4243,7 +4430,7 @@
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J74">
         <v>8</v>
@@ -4287,7 +4474,7 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J75">
         <v>8</v>
@@ -4331,7 +4518,7 @@
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J76">
         <v>8</v>
@@ -4375,7 +4562,7 @@
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J77">
         <v>8</v>
@@ -4419,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="I78" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J78">
         <v>8</v>
@@ -4439,15 +4626,15 @@
     </row>
     <row r="115" spans="5:9">
       <c r="E115" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="I115" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="5:9">
       <c r="E116" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -4464,10 +4651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:P200"/>
+  <dimension ref="A1:Q200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E205" sqref="E205"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4477,34 +4664,34 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="19" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="19" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -4519,7 +4706,7 @@
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="H6" s="19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I6" s="19"/>
     </row>
@@ -4530,55 +4717,55 @@
     </row>
     <row r="8" spans="1:16" ht="71" thickBot="1">
       <c r="A8" s="18" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="16" thickTop="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>11</v>
       </c>
@@ -4610,7 +4797,7 @@
         <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>8</v>
@@ -4660,7 +4847,7 @@
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>8</v>
@@ -4710,7 +4897,7 @@
         <v>8</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>8</v>
@@ -4760,7 +4947,7 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>8</v>
@@ -4810,7 +4997,7 @@
         <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>8</v>
@@ -4860,7 +5047,7 @@
         <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L14">
         <v>8</v>
@@ -4878,60 +5065,65 @@
         <v>256</v>
       </c>
     </row>
-    <row r="36" spans="3:10">
+    <row r="36" spans="3:17">
       <c r="C36" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17">
       <c r="D37" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="G37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="3:17">
       <c r="G38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="3:17">
       <c r="D40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="3:17">
       <c r="D41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="3:17">
       <c r="D42" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="3:17">
       <c r="D43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="3:17">
       <c r="C45" s="19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="3:10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17">
       <c r="I47" s="19" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J47" s="19"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="48" spans="3:17" ht="56">
+      <c r="Q48" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49">
         <v>1</v>
       </c>
@@ -4963,7 +5155,7 @@
         <v>8</v>
       </c>
       <c r="K49" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L49">
         <v>8</v>
@@ -4980,8 +5172,11 @@
       <c r="P49">
         <v>256</v>
       </c>
-    </row>
-    <row r="50" spans="1:16">
+      <c r="Q49" s="6">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50">
         <v>1</v>
       </c>
@@ -5013,7 +5208,7 @@
         <v>8</v>
       </c>
       <c r="K50" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="L50">
         <v>8</v>
@@ -5030,8 +5225,11 @@
       <c r="P50">
         <v>256</v>
       </c>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="Q50" s="6">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51">
         <v>1</v>
       </c>
@@ -5063,7 +5261,7 @@
         <v>8</v>
       </c>
       <c r="K51" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L51">
         <v>8</v>
@@ -5080,8 +5278,11 @@
       <c r="P51">
         <v>256</v>
       </c>
-    </row>
-    <row r="52" spans="1:16">
+      <c r="Q51" s="6">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52">
         <v>1</v>
       </c>
@@ -5113,7 +5314,7 @@
         <v>8</v>
       </c>
       <c r="K52" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L52">
         <v>8</v>
@@ -5130,8 +5331,11 @@
       <c r="P52">
         <v>256</v>
       </c>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="Q52" s="6">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53">
         <v>1</v>
       </c>
@@ -5163,7 +5367,7 @@
         <v>8</v>
       </c>
       <c r="K53" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="L53">
         <v>8</v>
@@ -5180,8 +5384,11 @@
       <c r="P53">
         <v>256</v>
       </c>
-    </row>
-    <row r="54" spans="1:16">
+      <c r="Q53" s="6">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
       <c r="A54">
         <v>1</v>
       </c>
@@ -5213,7 +5420,7 @@
         <v>8</v>
       </c>
       <c r="K54" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L54">
         <v>8</v>
@@ -5233,7 +5440,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="I75" s="19" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:16">
@@ -5268,7 +5475,7 @@
         <v>8</v>
       </c>
       <c r="K77" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L77">
         <v>8</v>
@@ -5318,7 +5525,7 @@
         <v>8</v>
       </c>
       <c r="K78" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L78">
         <v>8</v>
@@ -5368,7 +5575,7 @@
         <v>8</v>
       </c>
       <c r="K79" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L79">
         <v>8</v>
@@ -5418,7 +5625,7 @@
         <v>8</v>
       </c>
       <c r="K80" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L80">
         <v>8</v>
@@ -5468,7 +5675,7 @@
         <v>8</v>
       </c>
       <c r="K81" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L81">
         <v>8</v>
@@ -5488,7 +5695,7 @@
     </row>
     <row r="104" spans="1:16">
       <c r="I104" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106" spans="1:16">
@@ -5523,7 +5730,7 @@
         <v>8</v>
       </c>
       <c r="K106" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L106">
         <v>8</v>
@@ -5573,7 +5780,7 @@
         <v>8</v>
       </c>
       <c r="K107" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L107">
         <v>8</v>
@@ -5623,7 +5830,7 @@
         <v>8</v>
       </c>
       <c r="K108" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L108">
         <v>8</v>
@@ -5673,7 +5880,7 @@
         <v>8</v>
       </c>
       <c r="K109" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L109">
         <v>8</v>
@@ -5723,7 +5930,7 @@
         <v>8</v>
       </c>
       <c r="K110" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L110">
         <v>8</v>
@@ -5743,17 +5950,17 @@
     </row>
     <row r="130" spans="1:16">
       <c r="E130" s="21" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:16">
       <c r="F131" s="21" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="132" spans="1:16">
       <c r="G132" s="21" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="1:16">
@@ -5764,10 +5971,10 @@
     </row>
     <row r="135" spans="1:16">
       <c r="I135" s="19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K135" s="20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="136" spans="1:16" ht="16" customHeight="1"/>
@@ -5803,7 +6010,7 @@
         <v>8</v>
       </c>
       <c r="K137" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L137">
         <v>1</v>
@@ -5853,7 +6060,7 @@
         <v>8</v>
       </c>
       <c r="K138" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L138">
         <v>2</v>
@@ -5903,7 +6110,7 @@
         <v>8</v>
       </c>
       <c r="K139" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L139">
         <v>3</v>
@@ -5953,7 +6160,7 @@
         <v>8</v>
       </c>
       <c r="K140" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L140">
         <v>4</v>
@@ -6003,7 +6210,7 @@
         <v>8</v>
       </c>
       <c r="K141" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L141">
         <v>5</v>
@@ -6053,7 +6260,7 @@
         <v>8</v>
       </c>
       <c r="K142" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L142">
         <v>6</v>
@@ -6103,7 +6310,7 @@
         <v>8</v>
       </c>
       <c r="K143" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L143">
         <v>7</v>
@@ -6153,7 +6360,7 @@
         <v>8</v>
       </c>
       <c r="K144" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L144">
         <v>8</v>
@@ -6173,22 +6380,22 @@
     </row>
     <row r="165" spans="1:16">
       <c r="E165" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
     </row>
     <row r="166" spans="1:16">
       <c r="E166" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
     </row>
     <row r="167" spans="1:16">
       <c r="E167" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
     </row>
     <row r="170" spans="1:16">
       <c r="I170" s="19" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="172" spans="1:16">
@@ -6223,7 +6430,7 @@
         <v>8</v>
       </c>
       <c r="K172" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L172">
         <v>8</v>
@@ -6273,7 +6480,7 @@
         <v>8</v>
       </c>
       <c r="K173" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L173">
         <v>8</v>
@@ -6323,7 +6530,7 @@
         <v>8</v>
       </c>
       <c r="K174" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L174">
         <v>8</v>
@@ -6373,7 +6580,7 @@
         <v>8</v>
       </c>
       <c r="K175" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L175">
         <v>8</v>
@@ -6423,7 +6630,7 @@
         <v>8</v>
       </c>
       <c r="K176" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L176">
         <v>8</v>
@@ -6473,7 +6680,7 @@
         <v>8</v>
       </c>
       <c r="K177" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L177">
         <v>8</v>
@@ -6523,7 +6730,7 @@
         <v>8</v>
       </c>
       <c r="K178" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L178">
         <v>8</v>
@@ -6543,20 +6750,21 @@
     </row>
     <row r="198" spans="6:6">
       <c r="F198" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="199" spans="6:6">
       <c r="F199" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="200" spans="6:6">
       <c r="F200" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6581,16 +6789,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="49" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="9"/>
@@ -6609,10 +6817,10 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="8" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="12"/>
@@ -6653,31 +6861,31 @@
     </row>
     <row r="4" spans="1:18" ht="71" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -6923,7 +7131,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -7047,16 +7255,16 @@
     </row>
     <row r="18" spans="1:18" ht="49" thickBot="1">
       <c r="A18" s="7" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="9"/>
@@ -7075,10 +7283,10 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="12"/>
@@ -7119,31 +7327,31 @@
     </row>
     <row r="21" spans="1:18" ht="71" thickBot="1">
       <c r="A21" s="7" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -7295,10 +7503,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -7363,19 +7571,19 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N51">
         <v>2</v>
@@ -7419,19 +7627,19 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J52" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="K52" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="L52" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M52" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N52">
         <v>2</v>
@@ -7475,19 +7683,19 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J53" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K53" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L53" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M53" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N53">
         <v>2</v>
@@ -7531,19 +7739,19 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J54" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="K54" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="L54" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M54" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N54">
         <v>2</v>
@@ -7587,19 +7795,19 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J55" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="K55" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="L55" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M55" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N55">
         <v>2</v>
@@ -7643,19 +7851,19 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="J56" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="K56" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="L56" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="M56" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="N56">
         <v>2</v>
@@ -7674,7 +7882,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7698,7 +7905,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="E1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -7733,7 +7940,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L3">
         <v>8</v>
@@ -7783,7 +7990,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L4">
         <v>8</v>
@@ -7833,7 +8040,7 @@
         <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L5">
         <v>8</v>
@@ -7883,7 +8090,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L6">
         <v>8</v>
@@ -7933,7 +8140,7 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L7">
         <v>8</v>
@@ -7983,7 +8190,7 @@
         <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L8">
         <v>8</v>
@@ -8033,7 +8240,7 @@
         <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L9">
         <v>8</v>
@@ -8083,7 +8290,7 @@
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L10">
         <v>8</v>
@@ -8133,7 +8340,7 @@
         <v>8</v>
       </c>
       <c r="K18" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L18">
         <v>8</v>
@@ -8152,7 +8359,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>